<commit_message>
Further iteration on the model: removed the 'mode' slot (since the content of the TestSuite slot usage could infer mode); cleaned up and regenerated the project artifacts; validated testing (requires further elaboration!)
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -506,131 +506,115 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>test_metadata</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>test_persona</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>test_case_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>test_cases</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_case_specification</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_case_specification</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enumerated,Generated"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>test_case_specification</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enumerated,Generated"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1166,6 +1150,93 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1177,31 +1248,143 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_case_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>inputs</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>outputs</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_case_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
@@ -1213,245 +1396,10 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enumerated,Generated"</formula1>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>test_case_specification</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enumerated,Generated"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>inputs</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>outputs</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enumerated,Generated"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>test_case_specification</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enumerated,Generated"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 'tags' slot in TestEntity for global availability to 'mark up' assets; specified a TestAssetCollection a.k.a. Jenn's 'Block List' in disguise
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -9,21 +9,22 @@
   <sheets>
     <sheet name="TestMetadata" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="TestAsset" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="QueryAnswerPair" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TestEdgeData" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="TestCase" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TestCaseSpecification" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="TestSuite" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AcceptanceTestCase" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AcceptanceTestSuite" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="BenchmarkTestSuite" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="OneHopTestSuite" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Input" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="SemanticSmokeTestInput" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Output" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SemanticSmokeTestOutput" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Precondition" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="TestAssetCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="QueryAnswerPair" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TestEdgeData" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TestCase" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TestCaseSpecification" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="TestSuite" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AcceptanceTestCase" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="AcceptanceTestSuite" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="BenchmarkTestSuite" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="OneHopTestSuite" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Input" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="SemanticSmokeTestInput" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Output" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SemanticSmokeTestOutput" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Precondition" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +467,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -488,25 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,6 +536,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -561,13 +554,31 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +620,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -628,32 +644,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_case_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -664,7 +710,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -741,6 +828,11 @@
       <c r="N1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -760,70 +852,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -838,28 +899,74 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -874,7 +981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,6 +1048,11 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -966,7 +1078,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1033,6 +1191,11 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -1052,13 +1215,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,6 +1288,11 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -1144,13 +1312,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1189,40 +1357,9 @@
           <t>description</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -1237,7 +1374,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,6 +1457,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>
@@ -1292,13 +1475,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1337,69 +1520,13 @@
           <t>description</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_case_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial iteration on model normalization
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -9,22 +9,21 @@
   <sheets>
     <sheet name="TestMetadata" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="TestAsset" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestAssetCollection" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="QueryAnswerPair" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="TestEdgeData" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TestCase" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="TestCaseSpecification" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="TestSuite" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AcceptanceTestCase" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="AcceptanceTestSuite" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="BenchmarkTestSuite" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="OneHopTestSuite" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Input" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="SemanticSmokeTestInput" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Output" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="SemanticSmokeTestOutput" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Precondition" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="AcceptanceTestAsset" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TestEdgeData" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TestCase" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TestCaseSpecification" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AcceptanceTestCase" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="QuantitativeTestCase" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ComplianceTestCase" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="KnowledgeGraphNavigationTestCase" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="OneHopTestCase" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="TestSuite" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="AcceptanceTestSuite" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="BenchmarkTestSuite" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="OneHopTestSuite" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Precondition" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -494,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,49 +504,60 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>test_case_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_case_specification</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="3">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -560,14 +570,73 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -710,7 +779,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,37 +808,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_case_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -762,133 +874,51 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>must_pass_date</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>must_pass_environment</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>query</t>
+          <t>test_cases</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>string_entry</t>
+          <t>test_case_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>direction</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>answer_informal_concept</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>expected_result</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>curie</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>top_level</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>node</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"DEV,CI,TEST,PROD"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"increased,decreased"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"include_good,exclude_bad"</formula1>
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -934,7 +964,452 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>expected_output</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_issue</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>semantic_severity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>in_v1</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>well_known</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"High,Low,NotApplicable"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>must_pass_date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>must_pass_environment</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>query</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>string_entry</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>direction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>answer_informal_concept</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>expected_result</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>top_level</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>query_node</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>input_name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>output_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>expected_output</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>test_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>semantic_severity</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_v1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>well_known</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="7">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"increased,decreased"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"include_good,exclude_bad"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"subject,object"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"High,Low,NotApplicable"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>expected_output</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_issue</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>semantic_severity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>in_v1</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>well_known</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"High,Low,NotApplicable"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -975,13 +1450,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -992,65 +1467,45 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input_id</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>input_name</t>
+          <t>test_case_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>output_id</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>output_name</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>expected_output</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>test_issue</t>
+          <t>id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>semantic_severity</t>
+          <t>name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>in_v1</t>
+          <t>description</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>well_known</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1058,27 +1513,27 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"High,Low,NotApplicable"</formula1>
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1089,42 +1544,73 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>test_assets</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,65 +1621,45 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input_id</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>input_name</t>
+          <t>test_case_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>output_id</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>output_name</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>expected_output</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>test_issue</t>
+          <t>id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>semantic_severity</t>
+          <t>name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>in_v1</t>
+          <t>description</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>well_known</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1201,332 +1667,16 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"High,Low,NotApplicable"</formula1>
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>expected_output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>test_issue</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>semantic_severity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>in_v1</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>well_known</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"High,Low,NotApplicable"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>inputs</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>outputs</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_case_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>inputs</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>outputs</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add a quick and dirty script to generate test assets and cases from unstructured spreadsheet of data from P/F testing group.
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -1053,10 +1053,10 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
+      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
@@ -1217,10 +1217,10 @@
       <formula1>"subject,object"</formula1>
     </dataValidation>
     <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
+      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
     <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
     <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
@@ -1319,10 +1319,10 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,1_TopAnswer,4_NeverShow"</formula1>
+      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles"</formula1>
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>

</xml_diff>

<commit_message>
update to include 'settings'
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -970,7 +970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1031,20 +1031,25 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>runner_settings</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1072,7 +1077,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1183,20 +1188,25 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
+          <t>runner_settings</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1236,7 +1246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1297,20 +1307,25 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>runner_settings</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>

</xml_diff>

<commit_message>
Regenerate model artifacts to include model tweaks from commits
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -970,7 +970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1031,25 +1031,30 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_reference</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1077,7 +1082,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1188,25 +1193,30 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
+          <t>test_reference</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1246,7 +1256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,25 +1317,30 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_reference</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>

</xml_diff>

<commit_message>
Significant iteration in the design & basic stub implementation of a novel TestCaseGenerator class facade for accessing TestCase instances in the TestHarness
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -11,8 +11,8 @@
     <sheet name="TestAsset" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="AcceptanceTestAsset" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="TestEdgeData" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="TestCase" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TestCaseSpecification" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Precondition" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TestCase" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="AcceptanceTestCase" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="QuantitativeTestCase" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="ComplianceTestCase" sheetId="9" state="visible" r:id="rId9"/>
@@ -23,7 +23,7 @@
     <sheet name="BenchmarkTestSuite" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="StandardsComplianceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="OneHopTestSuite" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Precondition" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="TestSuiteSpecification" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,54 +509,46 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case_type</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
@@ -570,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,54 +578,46 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case_type</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
@@ -673,7 +657,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_case_specification</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -739,7 +723,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_case_specification</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -823,7 +807,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_case_specification</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -889,7 +873,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_case_specification</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -929,7 +913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -940,26 +924,41 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>test_data_file_locator</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_data_file_format</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"TSV,YAML,JSON"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1368,83 +1367,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_case_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1480,13 +1402,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1502,54 +1424,46 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case_type</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1557,13 +1471,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1579,54 +1493,46 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case_type</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1634,13 +1540,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1656,54 +1562,115 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case_type</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"acceptance,quantitative,compliance,kg_navigation,one_hop"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Another quick iteration on an abstract TestRunner interface
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -24,6 +24,7 @@
     <sheet name="StandardsComplianceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="OneHopTestSuite" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="TestSuiteSpecification" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="TestCaseResult" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -963,6 +964,72 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_suite_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_case_result</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"test_passed,test_failed,test_skipped"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
add more meta data to TestCase generation, generate cases from benchmark metadata
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,27 +529,37 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -558,6 +568,12 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -570,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,27 +622,37 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -635,6 +661,12 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1353,7 +1385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1389,27 +1421,37 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -1418,6 +1460,12 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1471,7 +1519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1507,27 +1555,37 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -1536,6 +1594,12 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1548,7 +1612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1584,27 +1648,37 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -1613,6 +1687,12 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1625,7 +1705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1661,27 +1741,37 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -1690,6 +1780,12 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fleshing out TestRunner unit tests using mock data; iterating on a stub implementation of the run() method
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -444,12 +444,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>parameter</t>
+          <t>parameter_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>parameter_value</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhancing the TestAsset class to include addition (optional) slots which reflect full Biolink Model association ("edge") semantics including node and edge categories with qualifiers
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -464,7 +464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,50 +475,60 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>trapi_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biolink_version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>test_env</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>query_type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>test_assets</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>preconditions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>trapi_template</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>components</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -526,16 +536,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1294,7 +1304,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1315,70 +1325,90 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>predicate</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>association</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>test_issue</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>semantic_severity</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>in_v1</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>well_known</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>test_reference</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1386,13 +1416,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1406,7 +1436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1477,70 +1507,90 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>predicate</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>output_id</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>association</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>test_issue</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>semantic_severity</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>in_v1</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>well_known</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>test_reference</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1560,13 +1610,13 @@
     <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"subject,object"</formula1>
     </dataValidation>
-    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="T2:T1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
-    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
-    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="V2:V1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1580,7 +1630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1601,70 +1651,90 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>predicate</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>association</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>test_issue</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>semantic_severity</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>in_v1</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>well_known</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>test_reference</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1672,13 +1742,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Additional iteration with some renaming of classes and slots to be more consistent, both with the Biolink Model and with the nomenclature of the testing model itself.
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -8,26 +8,27 @@
   </bookViews>
   <sheets>
     <sheet name="TestEntityParameter" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TestMetadata" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestAsset" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="AcceptanceTestAsset" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="TestEdgeData" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Precondition" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="TestCase" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AcceptanceTestCase" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="QuantitativeTestCase" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="ComplianceTestCase" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="KnowledgeGraphNavigationTestCase" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="OneHopTestCase" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="TestSuiteSpecification" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="TestSuite" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AcceptanceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="BenchmarkTestSuite" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="OneHopTestSuite" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="TestRunnerConfiguration" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="TestCaseResult" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="TestRunSession" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Qualifier" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TestMetadata" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TestAsset" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="AcceptanceTestAsset" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TestEdgeData" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Precondition" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="TestCase" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AcceptanceTestCase" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="QuantitativeTestCase" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ComplianceTestCase" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="KnowledgeGraphNavigationTestCase" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="OneHopTestCase" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="TestSuiteSpecification" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="TestSuite" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AcceptanceTestSuite" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="BenchmarkTestSuite" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="OneHopTestSuite" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="TestRunnerConfiguration" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="TestCaseResult" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TestRunSession" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -464,6 +465,91 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -546,91 +632,6 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
   </dataValidations>
@@ -729,6 +730,91 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -773,72 +859,6 @@
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"TSV,YAML,JSON"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_suite_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -917,24 +937,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -991,6 +993,24 @@
       <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1067,6 +1087,103 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>parameter</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1107,7 +1224,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_suite_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_case_result</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"test_passed,test_failed,test_skipped"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1124,22 +1302,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_source</t>
+          <t>test_runner_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_reference</t>
+          <t>test_entities</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_objective</t>
+          <t>test_case_results</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_annotations</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1164,80 +1342,11 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_suite_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_case</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_case_result</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"test_passed,test_failed,test_skipped"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1254,22 +1363,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_runner_name</t>
+          <t>test_source</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_entities</t>
+          <t>test_reference</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_case_results</t>
+          <t>test_objective</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>test_annotations</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1294,17 +1403,25 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1330,85 +1447,90 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>predicate</t>
+          <t>predicate_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>predicate_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>output_id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>output_category</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>association</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>qualifiers</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>test_issue</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>semantic_severity</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>in_v1</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>well_known</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>test_reference</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1416,13 +1538,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
-    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
-    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1430,13 +1552,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1512,85 +1634,90 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>predicate</t>
+          <t>predicate_id</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
+          <t>predicate_name</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
           <t>output_id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>output_category</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>association</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>qualifiers</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>test_issue</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>semantic_severity</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>in_v1</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>well_known</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>test_reference</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1610,13 +1737,13 @@
     <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"subject,object"</formula1>
     </dataValidation>
-    <dataValidation sqref="T2:T1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
-    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="V2:V1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
-    <dataValidation sqref="V2:V1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="W2:W1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1624,13 +1751,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1656,85 +1783,90 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>predicate</t>
+          <t>predicate_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>predicate_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>output_id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>output_category</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>association</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>qualifiers</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>test_issue</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>semantic_severity</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>in_v1</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>well_known</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>test_reference</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>runner_settings</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1742,13 +1874,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
     </dataValidation>
-    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
-    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"High,Low,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1756,7 +1888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1793,91 +1925,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix script to group assets into cases
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -28,6 +28,8 @@
     <sheet name="TestRunnerConfiguration" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="TestCaseResult" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="TestRunSession" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TestOutput" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TestResultPKSet" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1288,13 +1290,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P1"/>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1305,6 +1307,138 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>test_suite_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>pks</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>parent_pk</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>merged_pk</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>aragorn</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>arax</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unsecret</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>bte</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>improving</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>input_id</t>
         </is>
       </c>
@@ -1365,20 +1499,25 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1387,7 +1526,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
+      <formula1>"Acceptable,BadButForgivable,NeverShow,TopAnswer"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
@@ -1406,7 +1545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1527,20 +1666,25 @@
       </c>
       <c r="W1" t="inlineStr">
         <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1561,7 +1705,7 @@
       <formula1>"subject,object"</formula1>
     </dataValidation>
     <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
+      <formula1>"Acceptable,BadButForgivable,NeverShow,TopAnswer"</formula1>
     </dataValidation>
     <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
@@ -1580,7 +1724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1651,20 +1795,25 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1673,7 +1822,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Top_Answer,Acceptable,BadButForgivable,NeverShow,number_1_TopAnswer,number_2_Acceptable,number_3_BadButForgivable,number_4_NeverShow"</formula1>
+      <formula1>"Acceptable,BadButForgivable,NeverShow,TopAnswer"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>

</xml_diff>

<commit_message>
regenerate project to fix conflicts
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -1296,7 +1296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,35 +1307,30 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_suite_id</t>
+          <t>test_case_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case</t>
+          <t>pks</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>pks</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>

</xml_diff>

<commit_message>
fix up schema so benchmarks can comply
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,27 +508,37 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -540,6 +550,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -547,6 +563,117 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>trapi_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biolink_version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -563,42 +690,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>trapi_version</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biolink_version</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>components</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -623,31 +750,37 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+  <dataValidations count="6">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -688,27 +821,37 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -721,90 +864,11 @@
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"arax,aragorn,ars,bte,improving"</formula1>
     </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1671,10 +1735,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Acceptable,BadButForgivable,NeverShow,TopAnswer"</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
@@ -1863,7 +1924,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -1875,9 +1936,6 @@
     </dataValidation>
     <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"subject,object"</formula1>
-    </dataValidation>
-    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Acceptable,BadButForgivable,NeverShow,TopAnswer"</formula1>
     </dataValidation>
     <dataValidation sqref="V2:V1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
@@ -2017,10 +2075,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Acceptable,BadButForgivable,NeverShow,TopAnswer"</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
     </dataValidation>
@@ -2079,7 +2134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2120,27 +2175,37 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -2152,6 +2217,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2164,7 +2235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2205,27 +2276,37 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
@@ -2237,6 +2318,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add redundant fields to TestCase per feedback
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,20 +518,30 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>test_case_predicate</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -563,6 +573,127 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>trapi_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biolink_version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>test_case_predicate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -579,52 +710,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>trapi_version</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biolink_version</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>components</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
@@ -650,22 +781,22 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+    </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -673,13 +804,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,121 +861,30 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>test_case_predicate</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2134,7 +2174,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2185,20 +2225,30 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>test_case_predicate</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2235,7 +2285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2286,20 +2336,30 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>test_case_predicate</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>

</xml_diff>

<commit_message>
adding space for qualifiers
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -569,7 +569,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
@@ -700,7 +700,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
@@ -821,7 +821,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
@@ -942,7 +942,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
@@ -1694,7 +1694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1795,20 +1795,45 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>biolink_qualified_predicate</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>biolink_subject_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>biolink_subject_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>biolink_object_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>biolink_object_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1833,7 +1858,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1984,20 +2009,45 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
+          <t>biolink_qualified_predicate</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>biolink_subject_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>biolink_subject_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>biolink_object_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>biolink_object_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2034,7 +2084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2135,20 +2185,45 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>biolink_qualified_predicate</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>biolink_subject_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>biolink_subject_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>biolink_object_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>biolink_object_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2316,7 +2391,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
@@ -2437,7 +2512,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>

</xml_diff>

<commit_message>
Added OneHopTests and StandardsValidation to TestObjectiveEnum; regenerate artifacts
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -569,10 +569,10 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -700,10 +700,10 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -821,10 +821,10 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -942,10 +942,10 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -1681,7 +1681,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2316,10 +2316,10 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -2437,10 +2437,10 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"arax,aragorn,ars,bte,improving"</formula1>
+      <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>

</xml_diff>

<commit_message>
Subclass KnowledgeGraphNavigationTestCase from ComplianceTestCase
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -719,7 +719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,80 +730,90 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>trapi_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biolink_version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>test_env</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>query_type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>test_assets</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>preconditions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>trapi_template</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>components</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>test_case_objective</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>test_case_source</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>test_case_predicate_name</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>test_case_predicate_id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -811,22 +821,22 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -840,7 +850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,80 +861,90 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>trapi_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biolink_version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>test_env</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>query_type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>test_assets</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>preconditions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>trapi_template</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>components</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>test_case_objective</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>test_case_source</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>test_case_predicate_name</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>test_case_predicate_id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -932,22 +952,22 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Refactored runner_settings into test_run_settings inside TestEntity; simplified global TestRunner tag=value configuration as TestRunSession.test_run_parameters slot; further documented usage in a few places; removed some TestCase subclasses that felt superfluous given the aforementioned TestRunner configuration changes.
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -17,20 +17,16 @@
     <sheet name="TestCase" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="AcceptanceTestCase" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="QuantitativeTestCase" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="ComplianceTestCase" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="KnowledgeGraphNavigationTestCase" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="OneHopTestCase" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="TestSuiteSpecification" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="TestSuite" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AcceptanceTestSuite" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="BenchmarkTestSuite" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="OneHopTestSuite" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="TestRunnerConfiguration" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="TestCaseResult" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="TestRunSession" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="TestOutput" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="TestResultPKSet" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TestSuiteSpecification" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="TestSuite" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="AcceptanceTestSuite" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="BenchmarkTestSuite" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="OneHopTestSuite" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="TestCaseResult" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="TestRunSession" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="TestOutput" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="TestResultPKSet" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,103 +474,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_predicate_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>test_case_input_id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>test_case_runner_settings</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="4">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -588,7 +568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,114 +579,44 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>trapi_version</t>
+          <t>test_data_file_locator</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biolink_version</t>
+          <t>test_data_file_format</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_case_runner_settings</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"TSV,YAML,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -719,7 +629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,114 +640,54 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>trapi_version</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biolink_version</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>test_cases</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_case_runner_settings</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -850,7 +700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,114 +711,54 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>trapi_version</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biolink_version</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>test_cases</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_case_runner_settings</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -981,7 +771,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -992,46 +800,132 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_data_file_locator</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_data_file_format</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"TSV,YAML,JSON"</formula1>
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1048,62 +942,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>test_suite_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>test_case</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>test_case_result</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_suite_specification</t>
+          <t>id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"test_passed,test_failed,test_skipped"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1114,80 +1008,85 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>components</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>test_runner_name</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_suite_specification</t>
+          <t>test_run_parameters</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>test_entities</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>test_case_results</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1198,117 +1097,41 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>test_case_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>pks</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_suite_specification</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_suite_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1350,7 +1173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1361,27 +1184,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_run_parameters</t>
+          <t>parent_pk</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>merged_pk</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>aragorn</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>arax</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unsecret</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>bte</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>improving</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1390,13 +1248,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1407,291 +1265,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_suite_id</t>
+          <t>test_source</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case</t>
+          <t>test_reference</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_case_result</t>
+          <t>test_objective</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>test_annotations</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"test_passed,test_failed,test_skipped"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_runner_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_entities</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_case_results</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_case_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>pks</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>parent_pk</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>merged_pk</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>aragorn</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>arax</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unsecret</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>bte</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>improving</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_source</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_reference</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_objective</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_annotations</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1805,32 +1419,32 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>runner_settings</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>id</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1994,32 +1608,32 @@
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>runner_settings</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>id</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -2145,32 +1759,32 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>runner_settings</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>id</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -2193,7 +1807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2222,6 +1836,11 @@
           <t>tags</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2234,7 +1853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2245,103 +1864,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_predicate_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>test_case_input_id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>test_case_runner_settings</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="4">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2355,7 +1958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2366,103 +1969,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_predicate_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>test_case_input_id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>test_case_runner_settings</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="4">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixed TestObjectiveEnum values as per feedback from Max
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -552,7 +552,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -1315,7 +1315,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1942,7 +1942,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -2047,7 +2047,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTests,StandardsValidation"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>

</xml_diff>

<commit_message>
making a new release of TranslatorTesting Model
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -1694,7 +1694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1795,45 +1795,20 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>biolink_qualified_predicate</t>
+          <t>id</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>biolink_subject_aspect_qualifier</t>
+          <t>name</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>biolink_subject_direction_qualifier</t>
+          <t>description</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
-        <is>
-          <t>biolink_object_aspect_qualifier</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>biolink_object_direction_qualifier</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -1858,7 +1833,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2009,45 +1984,20 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>biolink_qualified_predicate</t>
+          <t>id</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>biolink_subject_aspect_qualifier</t>
+          <t>name</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>biolink_subject_direction_qualifier</t>
+          <t>description</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
-        <is>
-          <t>biolink_object_aspect_qualifier</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>biolink_object_direction_qualifier</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2084,7 +2034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2185,45 +2135,20 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>biolink_qualified_predicate</t>
+          <t>id</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>biolink_subject_aspect_qualifier</t>
+          <t>name</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>biolink_subject_direction_qualifier</t>
+          <t>description</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
-        <is>
-          <t>biolink_object_aspect_qualifier</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>biolink_object_direction_qualifier</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>

</xml_diff>

<commit_message>
Rationalize and expand testing model (#24)
* Added OneHopTests and StandardsValidation to TestObjectiveEnum
* Refactored runner_settings into test_run_settings inside TestEntity; simplified global TestRunner tag=value configuration as TestRunSession.test_run_parameters slot; further documented usage in a few places; removed some TestCase subclasses that felt superfluous given the aforementioned TestRunner configuration changes.
* Repaired example data to fix unit tests
* Fixed TestObjectiveEnum values as per feedback from Max
* regenerated project artifacts
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -17,20 +17,16 @@
     <sheet name="TestCase" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="AcceptanceTestCase" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="QuantitativeTestCase" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="ComplianceTestCase" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="KnowledgeGraphNavigationTestCase" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="OneHopTestCase" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="TestSuiteSpecification" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="TestSuite" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AcceptanceTestSuite" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="BenchmarkTestSuite" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="OneHopTestSuite" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="TestRunnerConfiguration" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="TestCaseResult" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="TestRunSession" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="TestOutput" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="TestResultPKSet" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TestSuiteSpecification" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="TestSuite" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="AcceptanceTestSuite" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="BenchmarkTestSuite" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="OneHopTestSuite" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="TestCaseResult" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="TestRunSession" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="TestOutput" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="TestResultPKSet" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,103 +474,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_predicate_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>test_case_input_id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>test_case_runner_settings</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="4">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -588,7 +568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,114 +579,44 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>trapi_version</t>
+          <t>test_data_file_locator</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biolink_version</t>
+          <t>test_data_file_format</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_case_runner_settings</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"TSV,YAML,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -719,7 +629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,104 +640,54 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>test_cases</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_case_runner_settings</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -840,7 +700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,104 +711,54 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>test_cases</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>test_suite_specification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_case_runner_settings</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -961,7 +771,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -972,46 +800,132 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_data_file_locator</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_data_file_format</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"TSV,YAML,JSON"</formula1>
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1028,62 +942,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>test_suite_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>test_case</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>test_case_result</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_suite_specification</t>
+          <t>id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"test_passed,test_failed,test_skipped"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1094,80 +1008,85 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>components</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>test_runner_name</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_suite_specification</t>
+          <t>test_run_parameters</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>test_entities</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>test_case_results</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1178,117 +1097,41 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>test_case_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_persona</t>
+          <t>pks</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_cases</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test_suite_specification</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_suite_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1330,7 +1173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1341,27 +1184,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_run_parameters</t>
+          <t>parent_pk</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>merged_pk</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>aragorn</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>arax</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unsecret</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>bte</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>improving</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>tags</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1370,13 +1248,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1387,291 +1265,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_suite_id</t>
+          <t>test_source</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case</t>
+          <t>test_reference</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_case_result</t>
+          <t>test_objective</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>test_annotations</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"test_passed,test_failed,test_skipped"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_runner_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_entities</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_case_results</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_case_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>pks</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>parent_pk</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>merged_pk</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>aragorn</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>arax</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unsecret</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>bte</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>improving</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_source</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_reference</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_objective</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_annotations</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1681,7 +1315,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1785,32 +1419,32 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>runner_settings</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>id</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1974,32 +1608,32 @@
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>runner_settings</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>id</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -2125,32 +1759,32 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>runner_settings</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>test_metadata</t>
+          <t>id</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -2173,7 +1807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2202,6 +1836,11 @@
           <t>tags</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2214,7 +1853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2225,103 +1864,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_predicate_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>test_case_input_id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>test_case_runner_settings</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="4">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2335,7 +1958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2346,103 +1969,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_env</t>
+          <t>query_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>preconditions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>trapi_template</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>components</t>
+          <t>test_case_source</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>test_case_predicate_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>test_case_predicate_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>test_case_input_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>test_case_input_id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>test_case_runner_settings</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>tags</t>
+          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="4">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update qualifiers on TestCase
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,30 +528,35 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_case_qualifiers</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -588,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,30 +664,35 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>test_case_qualifiers</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -719,7 +729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,30 +790,35 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_case_qualifiers</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -840,7 +855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -901,30 +916,35 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_case_qualifiers</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2214,7 +2234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2275,30 +2295,35 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_case_qualifiers</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
@@ -2335,7 +2360,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2396,30 +2421,35 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>test_case_qualifiers</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>test_case_input_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>test_case_runner_settings</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>

</xml_diff>

<commit_message>
update generator to produce just 1 and 4 asset suite
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,32 +534,42 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
@@ -571,6 +581,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1439,27 +1455,27 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>tags</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1628,27 +1644,27 @@
       </c>
       <c r="AB1" t="inlineStr">
         <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>tags</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1779,27 +1795,27 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>tags</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
         </is>
       </c>
     </row>
@@ -1868,7 +1884,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1939,32 +1955,42 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
@@ -1976,6 +2002,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1988,7 +2020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2059,32 +2091,42 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
@@ -2096,6 +2138,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
merge in work with updated schema, not using TestRun yet
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,32 +519,57 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
@@ -556,6 +581,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1853,7 +1884,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1909,32 +1940,57 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
@@ -1946,6 +2002,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1958,7 +2020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2014,32 +2076,57 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"treats"</formula1>
     </dataValidation>
@@ -2051,6 +2138,12 @@
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Small documentation update - test_objective descriptions, CONTRIBUTORS.md and in the makefile 'help' (#32)
* Clarified descriptions for **`StandardsValidationTest`** and **`OneHopTest`** values to **`test_objective`** Enum

* clarifying project instructions (both in the CONTRIBUTING.md document and the **`makefile help`**)

* regenerated project artifacts
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -577,7 +577,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -1346,7 +1346,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1998,7 +1998,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
@@ -2134,7 +2134,7 @@
       <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,OneHopTest,StandardsValidationTest"</formula1>
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>

</xml_diff>

<commit_message>
Converted the ComponentEnum to an explicit "permissible_values" Enum; cleaned up some unit test sample data tech debt
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -583,7 +583,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
@@ -1101,7 +1101,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
@@ -2004,7 +2004,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
@@ -2140,7 +2140,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>

</xml_diff>

<commit_message>
Move the pathfinder models to yaml
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -11,22 +11,24 @@
     <sheet name="Qualifier" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="TestMetadata" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="TestAsset" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="AcceptanceTestAsset" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TestEdgeData" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Precondition" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="TestCase" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AcceptanceTestCase" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="QuantitativeTestCase" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="TestSuiteSpecification" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="TestSuite" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="AcceptanceTestSuite" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="BenchmarkTestSuite" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="OneHopTestSuite" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="TestCaseResult" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="TestRunSession" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="TestOutput" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="TestResultPKSet" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="PathfinderTestAsset" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="AcceptanceTestAsset" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TestEdgeData" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Precondition" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="TestCase" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="PathfinderTestCase" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="AcceptanceTestCase" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="QuantitativeTestCase" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="TestSuiteSpecification" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="TestSuite" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AcceptanceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="BenchmarkTestSuite" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="OneHopTestSuite" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="TestCaseResult" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="TestRunSession" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="TestOutput" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TestResultPKSet" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -583,7 +585,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
@@ -594,6 +596,278 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -654,7 +928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -721,95 +995,6 @@
       <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_suite_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -891,6 +1076,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -956,7 +1159,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1018,151 +1292,6 @@
       <formula1>"PASSED,FAILED,SKIPPED"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_runner_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_run_parameters</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>test_entities</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>test_case_results</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_case_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>pks</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1215,6 +1344,151 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_runner_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_run_parameters</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_entities</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>test_case_results</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_case_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pks</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>parent_pk</t>
         </is>
       </c>
@@ -1498,6 +1772,185 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>source_input_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_input_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>source_input_category</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>target_input_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>target_input_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>target_input_category</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>path_nodes</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>minimum_required_path_nodes</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>input_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>input_name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>predicate_id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>predicate_name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>output_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>association</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>expected_output</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>test_issue</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>semantic_severity</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>in_v1</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>well_known</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>test_reference</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="T2:T1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
+    </dataValidation>
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"High,Low,NotApplicable"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1693,7 +2146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1832,7 +2285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1874,142 +2327,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>qualifiers</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>input_category</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>output_category</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
-    </dataValidation>
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2140,7 +2457,7 @@
       <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>

</xml_diff>

<commit_message>
Add performance test model and update pathfinder tests
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -10,25 +10,28 @@
     <sheet name="TestEntityParameter" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Qualifier" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="TestMetadata" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TestAsset" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="PathfinderTestAsset" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="AcceptanceTestAsset" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="TestEdgeData" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Precondition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="TestCase" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="PathfinderTestCase" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="AcceptanceTestCase" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="QuantitativeTestCase" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="TestSuiteSpecification" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="TestSuite" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AcceptanceTestSuite" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="BenchmarkTestSuite" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="StandardsComplianceTestSuite" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="OneHopTestSuite" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="TestCaseResult" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="TestRunSession" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="TestOutput" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="TestResultPKSet" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="PathfinderPathNode" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TestAsset" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="PathfinderTestAsset" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AcceptanceTestAsset" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="TestEdgeData" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Precondition" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="TestCase" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="PathfinderTestCase" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="AcceptanceTestCase" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="QuantitativeTestCase" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="PerformanceTestCase" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="TestSuiteSpecification" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="TestSuite" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="AcceptanceTestSuite" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="BenchmarkTestSuite" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="PerformanceTestSuite" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="StandardsComplianceTestSuite" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="OneHopTestSuite" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TestCaseResult" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TestRunSession" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="TestOutput" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TestResultPKSet" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -601,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,118 +615,59 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>query_type</t>
+          <t>test_assets</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_assets</t>
+          <t>test_case_objective</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>preconditions</t>
+          <t>components</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>trapi_template</t>
+          <t>test_env</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test_case_objective</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>test_case_source</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>test_case_predicate_name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>test_case_predicate_id</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>qualifiers</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>input_category</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>output_category</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
+  <dataValidations count="3">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
-    </dataValidation>
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"dev,ci,test,prod"</formula1>
     </dataValidation>
   </dataValidations>
@@ -873,6 +817,288 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_run_time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>spawn_rate</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>query_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_assets</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>trapi_template</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test_case_objective</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_case_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test_case_predicate_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>test_case_input_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>input_category</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>output_category</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>test_env</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"treats"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"dev,ci,test,prod"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -928,7 +1154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -995,95 +1221,6 @@
       <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_persona</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test_cases</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>test_suite_specification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1236,7 +1373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1247,40 +1384,45 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test_suite_id</t>
+          <t>test_metadata</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test_case</t>
+          <t>test_persona</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test_case_result</t>
+          <t>test_cases</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
@@ -1288,8 +1430,8 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"PASSED,FAILED,SKIPPED"</formula1>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1333,6 +1475,214 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_metadata</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_persona</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_cases</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test_suite_specification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"All,Clinical,LookUp,Mechanistic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_suite_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test_case</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test_case_result</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test_runner_settings</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"PASSED,FAILED,SKIPPED"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1416,7 +1766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1472,7 +1822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1633,6 +1983,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ids</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1766,13 +2147,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1813,139 +2194,61 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>predicate_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>predicate_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>minimum_required_path_nodes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>path_nodes</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>minimum_required_path_nodes</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>input_id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>input_name</t>
-        </is>
-      </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>input_category</t>
+          <t>expected_output</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>predicate_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>predicate_name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>output_id</t>
+          <t>description</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>output_name</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
-        <is>
-          <t>output_category</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>association</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>qualifiers</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>expected_output</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>test_issue</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>semantic_severity</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>in_v1</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>well_known</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>test_reference</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>test_metadata</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="T2:T1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"causes not treats,TMKP,category too generic,contraindications,chemical roles,test_issue"</formula1>
-    </dataValidation>
-    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"High,Low,NotApplicable"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2146,7 +2449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2285,7 +2588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2329,140 +2632,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>query_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test_assets</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>preconditions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>trapi_template</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>test_case_objective</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>test_case_source</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>test_case_predicate_id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>test_case_input_id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>qualifiers</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>input_category</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>output_category</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>components</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>test_env</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>tags</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>test_runner_settings</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"treats"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ameliorates,treats,three_hop,drug_treats_rare_disease,drug-to-gene"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"AcceptanceTest,BenchmarkTest,QuantitativeTest,StandardsValidationTest,OneHopTest"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SME,SMURF,GitHubUserFeedback,TACT,BenchMark,TranslatorTeam,TestDataLocation"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ars,arax,explanatory,improving,aragorn,bte,unsecret,rtxkg2,icees,cam,spoke,molepro,genetics,textmining,cohd,openpredict,collaboratory,connections"</formula1>
-    </dataValidation>
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"dev,ci,test,prod"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add qualifiers to pathfinder test asset
</commit_message>
<xml_diff>
--- a/project/excel/translator_testing_model.xlsx
+++ b/project/excel/translator_testing_model.xlsx
@@ -2153,7 +2153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2204,40 +2204,45 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>qualifiers</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>minimum_required_path_nodes</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>path_nodes</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>expected_output</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>test_runner_settings</t>
         </is>

</xml_diff>